<commit_message>
excel and invoice fixes
</commit_message>
<xml_diff>
--- a/public/uploads/order-import.xlsx
+++ b/public/uploads/order-import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu18.04\var\www\hd-v2\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA44557A-0712-44BB-9A11-1601C9DF5222}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021BBA0E-BBB5-40F8-8EA3-3107C4C466EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{AE4FF159-A0AA-4F60-8A11-073FF1539C6E}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>merchant</t>
   </si>
@@ -148,9 +148,6 @@
     <t>82huasd@mail.com</t>
   </si>
   <si>
-    <t>2238y283</t>
-  </si>
-  <si>
     <t>sakjdsd</t>
   </si>
   <si>
@@ -181,9 +178,6 @@
     <t>battery</t>
   </si>
   <si>
-    <t>flameable</t>
-  </si>
-  <si>
     <t>shoes</t>
   </si>
   <si>
@@ -194,13 +188,22 @@
   </si>
   <si>
     <t>kg/cm</t>
+  </si>
+  <si>
+    <t> +5518981424963</t>
+  </si>
+  <si>
+    <t>+5518981424963</t>
+  </si>
+  <si>
+    <t>Freight To Custom</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,6 +247,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -272,7 +281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -293,6 +302,15 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -610,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EE8AA69-184F-4EDD-986D-80D10476D1BA}">
   <dimension ref="A1:AF20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -620,13 +638,17 @@
     <col min="2" max="2" width="31.33203125" customWidth="1"/>
     <col min="3" max="3" width="34.88671875" customWidth="1"/>
     <col min="4" max="4" width="22.109375" customWidth="1"/>
-    <col min="5" max="19" width="15.6640625" customWidth="1"/>
+    <col min="5" max="12" width="15.6640625" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" style="10" customWidth="1"/>
+    <col min="14" max="16" width="15.6640625" customWidth="1"/>
+    <col min="17" max="17" width="20.109375" style="10" customWidth="1"/>
+    <col min="18" max="19" width="15.6640625" customWidth="1"/>
     <col min="20" max="20" width="20.88671875" customWidth="1"/>
-    <col min="21" max="27" width="15.6640625" customWidth="1"/>
-    <col min="28" max="28" width="25.88671875" customWidth="1"/>
-    <col min="29" max="29" width="21" customWidth="1"/>
-    <col min="30" max="30" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17" bestFit="1" customWidth="1"/>
+    <col min="21" max="28" width="15.6640625" customWidth="1"/>
+    <col min="29" max="29" width="25.88671875" customWidth="1"/>
+    <col min="30" max="30" width="21" style="10" customWidth="1"/>
+    <col min="31" max="31" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -646,7 +668,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
@@ -655,30 +677,30 @@
         <v>5</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="9" t="s">
         <v>8</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="9" t="s">
         <v>10</v>
       </c>
       <c r="R1" s="3" t="s">
@@ -706,25 +728,25 @@
         <v>18</v>
       </c>
       <c r="Z1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AB1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
@@ -753,7 +775,7 @@
         <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K2" t="s">
         <v>21</v>
@@ -761,8 +783,8 @@
       <c r="L2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M2">
-        <v>29863239389</v>
+      <c r="M2" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="N2" t="s">
         <v>23</v>
@@ -770,8 +792,8 @@
       <c r="P2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Q2">
-        <v>55128121288</v>
+      <c r="Q2" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="R2" t="s">
         <v>25</v>
@@ -794,16 +816,16 @@
       <c r="Y2">
         <v>98273982783</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>1</v>
       </c>
-      <c r="AA2">
+      <c r="AB2">
         <v>5</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>31</v>
       </c>
-      <c r="AC2">
+      <c r="AD2" s="10">
         <v>233847</v>
       </c>
     </row>
@@ -814,16 +836,16 @@
       <c r="F3" s="1"/>
       <c r="L3" s="2"/>
       <c r="P3" s="2"/>
-      <c r="Z3">
+      <c r="AA3">
         <v>2</v>
       </c>
-      <c r="AA3">
+      <c r="AB3">
         <v>1</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>31</v>
       </c>
-      <c r="AC3">
+      <c r="AD3" s="10">
         <v>233848</v>
       </c>
     </row>
@@ -834,20 +856,20 @@
       <c r="F4" s="1"/>
       <c r="L4" s="2"/>
       <c r="P4" s="2"/>
-      <c r="Z4">
+      <c r="AA4">
         <v>1</v>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <v>2</v>
       </c>
-      <c r="AB4" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC4">
+      <c r="AC4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD4" s="10">
         <v>233884</v>
       </c>
-      <c r="AD4" t="s">
-        <v>53</v>
+      <c r="AE4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
@@ -857,16 +879,16 @@
       <c r="F5" s="1"/>
       <c r="L5" s="2"/>
       <c r="P5" s="2"/>
-      <c r="Z5">
-        <v>1</v>
-      </c>
       <c r="AA5">
         <v>1</v>
       </c>
-      <c r="AB5" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC5">
+      <c r="AB5">
+        <v>1</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD5" s="10">
         <v>398744</v>
       </c>
     </row>
@@ -896,7 +918,7 @@
         <v>23</v>
       </c>
       <c r="I6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K6" t="s">
         <v>36</v>
@@ -904,7 +926,7 @@
       <c r="L6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="10">
         <v>2938998</v>
       </c>
       <c r="N6" t="s">
@@ -913,11 +935,11 @@
       <c r="P6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="Q6" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="R6" t="s">
         <v>40</v>
-      </c>
-      <c r="R6" t="s">
-        <v>41</v>
       </c>
       <c r="T6">
         <v>2323</v>
@@ -926,7 +948,7 @@
         <v>23243</v>
       </c>
       <c r="V6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W6" t="s">
         <v>27</v>
@@ -937,20 +959,20 @@
       <c r="Y6">
         <v>82973987</v>
       </c>
-      <c r="Z6">
+      <c r="AA6">
         <v>1</v>
       </c>
-      <c r="AA6">
+      <c r="AB6">
         <v>2</v>
       </c>
-      <c r="AB6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC6">
+      <c r="AC6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD6" s="10">
         <v>983434</v>
       </c>
-      <c r="AE6" t="s">
-        <v>53</v>
+      <c r="AF6" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
@@ -1013,7 +1035,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2:AF4" xr:uid="{5EA4B698-AE3D-433F-8CDD-F6223315DA05}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE2:AF4" xr:uid="{5EA4B698-AE3D-433F-8CDD-F6223315DA05}">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update upload files issue 339
</commit_message>
<xml_diff>
--- a/public/uploads/order-import.xlsx
+++ b/public/uploads/order-import.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t>merchant</t>
   </si>
@@ -48,12 +48,6 @@
     <t>width</t>
   </si>
   <si>
-    <t>sender_email</t>
-  </si>
-  <si>
-    <t>sender_phone</t>
-  </si>
-  <si>
     <t>recipient_email</t>
   </si>
   <si>
@@ -90,9 +84,6 @@
     <t>fedex</t>
   </si>
   <si>
-    <t>marcio</t>
-  </si>
-  <si>
     <t>marcio.feitas@gmail.com</t>
   </si>
   <si>
@@ -129,12 +120,6 @@
     <t>kalsdn</t>
   </si>
   <si>
-    <t>asdns</t>
-  </si>
-  <si>
-    <t>ssadfas@mail.cm</t>
-  </si>
-  <si>
     <t>kjasbdjb</t>
   </si>
   <si>
@@ -148,12 +133,6 @@
   </si>
   <si>
     <t>length</t>
-  </si>
-  <si>
-    <t>sender first_name</t>
-  </si>
-  <si>
-    <t>sender last name</t>
   </si>
   <si>
     <t>recipient first_name</t>
@@ -211,7 +190,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,12 +234,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF212529"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -289,7 +262,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -314,9 +287,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -634,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF20"/>
+  <dimension ref="A1:AB20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,23 +616,18 @@
     <col min="2" max="2" width="31.28515625" customWidth="1"/>
     <col min="3" max="3" width="34.85546875" customWidth="1"/>
     <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="15.7109375" customWidth="1"/>
-    <col min="17" max="17" width="20.140625" style="10" customWidth="1"/>
-    <col min="18" max="19" width="15.7109375" customWidth="1"/>
-    <col min="20" max="20" width="20.85546875" customWidth="1"/>
-    <col min="21" max="28" width="15.7109375" customWidth="1"/>
-    <col min="29" max="29" width="25.85546875" customWidth="1"/>
-    <col min="30" max="30" width="21" style="10" customWidth="1"/>
-    <col min="31" max="31" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" style="10" customWidth="1"/>
+    <col min="14" max="15" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="20.85546875" customWidth="1"/>
+    <col min="17" max="24" width="15.7109375" customWidth="1"/>
+    <col min="25" max="25" width="25.85546875" customWidth="1"/>
+    <col min="26" max="26" width="21" style="10" customWidth="1"/>
+    <col min="27" max="27" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -679,7 +644,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
@@ -688,13 +653,13 @@
         <v>5</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>7</v>
@@ -703,69 +668,57 @@
         <v>8</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="X1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="B2" t="s">
         <v>18</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
       </c>
       <c r="C2">
         <v>29873928</v>
@@ -786,132 +739,120 @@
         <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2">
+        <v>28937</v>
+      </c>
+      <c r="Q2">
+        <v>87272</v>
+      </c>
+      <c r="R2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="S2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2" t="s">
-        <v>55</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>23</v>
       </c>
-      <c r="T2">
-        <v>28937</v>
-      </c>
       <c r="U2">
-        <v>87272</v>
-      </c>
-      <c r="V2" t="s">
-        <v>24</v>
-      </c>
-      <c r="W2" t="s">
-        <v>25</v>
-      </c>
-      <c r="X2" t="s">
+        <v>98273982783</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>5</v>
+      </c>
+      <c r="Y2" t="s">
         <v>26</v>
       </c>
-      <c r="Y2">
-        <v>98273982783</v>
-      </c>
-      <c r="AA2">
-        <v>1</v>
-      </c>
-      <c r="AB2">
-        <v>5</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD2" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Z2" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>123132</v>
       </c>
       <c r="F3" s="1"/>
       <c r="L3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="AA3">
+      <c r="W3">
         <v>2</v>
       </c>
-      <c r="AB3">
+      <c r="X3">
         <v>1</v>
       </c>
-      <c r="AC3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD3" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Y3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z3" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>123132</v>
       </c>
       <c r="F4" s="1"/>
       <c r="L4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="AA4">
+      <c r="W4">
         <v>1</v>
       </c>
-      <c r="AB4">
+      <c r="X4">
         <v>2</v>
       </c>
-      <c r="AC4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD4" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Y4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>123132</v>
       </c>
       <c r="F5" s="1"/>
       <c r="L5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="AA5">
+      <c r="W5">
         <v>1</v>
       </c>
-      <c r="AB5">
+      <c r="X5">
         <v>1</v>
       </c>
-      <c r="AC5" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD5" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Y5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z5" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>13241324</v>
@@ -929,135 +870,110 @@
         <v>23</v>
       </c>
       <c r="I6" t="s">
-        <v>51</v>
-      </c>
-      <c r="K6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="N6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6">
+        <v>2323</v>
+      </c>
+      <c r="Q6">
+        <v>23243</v>
+      </c>
+      <c r="R6" t="s">
         <v>34</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="M6" s="10">
-        <v>2938998</v>
-      </c>
-      <c r="N6" t="s">
-        <v>36</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q6" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="R6" t="s">
-        <v>38</v>
-      </c>
-      <c r="T6">
-        <v>2323</v>
+      <c r="S6" t="s">
+        <v>22</v>
+      </c>
+      <c r="T6" t="s">
+        <v>23</v>
       </c>
       <c r="U6">
-        <v>23243</v>
-      </c>
-      <c r="V6" t="s">
-        <v>39</v>
-      </c>
-      <c r="W6" t="s">
-        <v>25</v>
-      </c>
-      <c r="X6" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y6">
         <v>82973987</v>
       </c>
-      <c r="AA6">
+      <c r="W6">
         <v>1</v>
       </c>
-      <c r="AB6">
+      <c r="X6">
         <v>2</v>
       </c>
-      <c r="AC6" t="s">
-        <v>47</v>
-      </c>
-      <c r="AD6" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Y6" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z6" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="L7" s="2"/>
-      <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="L8" s="2"/>
-      <c r="P8" s="2"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="L9" s="2"/>
-      <c r="P9" s="2"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="L10" s="2"/>
-      <c r="P10" s="2"/>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="L11" s="2"/>
-      <c r="P11" s="2"/>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="L12" s="2"/>
-      <c r="P12" s="2"/>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="L13" s="2"/>
-      <c r="P13" s="2"/>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="L14" s="2"/>
-      <c r="P14" s="2"/>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="L15" s="2"/>
-      <c r="P15" s="2"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="L16" s="2"/>
-      <c r="P16" s="2"/>
-    </row>
-    <row r="17" spans="12:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L17" s="2"/>
-      <c r="P17" s="2"/>
-    </row>
-    <row r="18" spans="12:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L18" s="2"/>
-      <c r="P18" s="2"/>
-    </row>
-    <row r="19" spans="12:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L19" s="2"/>
-      <c r="P19" s="2"/>
-    </row>
-    <row r="20" spans="12:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L20" s="2"/>
-      <c r="P20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE2:AF4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2:AB4">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-    <hyperlink ref="L6" r:id="rId2"/>
-    <hyperlink ref="P6" r:id="rId3"/>
-    <hyperlink ref="P2" r:id="rId4"/>
+    <hyperlink ref="L6" r:id="rId1"/>
+    <hyperlink ref="L2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update upload files updated sample
</commit_message>
<xml_diff>
--- a/public/uploads/order-import.xlsx
+++ b/public/uploads/order-import.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu18.04\var\www\hd-v2\public\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\hd-v2\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021BBA0E-BBB5-40F8-8EA3-3107C4C466EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{AE4FF159-A0AA-4F60-8A11-073FF1539C6E}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>merchant</t>
   </si>
@@ -49,12 +48,6 @@
     <t>width</t>
   </si>
   <si>
-    <t>sender_email</t>
-  </si>
-  <si>
-    <t>sender_phone</t>
-  </si>
-  <si>
     <t>recipient_email</t>
   </si>
   <si>
@@ -91,12 +84,6 @@
     <t>fedex</t>
   </si>
   <si>
-    <t>marcio</t>
-  </si>
-  <si>
-    <t>marcio.feitas@gmail.com</t>
-  </si>
-  <si>
     <t>saqib</t>
   </si>
   <si>
@@ -136,12 +123,6 @@
     <t>kalsdn</t>
   </si>
   <si>
-    <t>asdns</t>
-  </si>
-  <si>
-    <t>ssadfas@mail.cm</t>
-  </si>
-  <si>
     <t>kjasbdjb</t>
   </si>
   <si>
@@ -155,12 +136,6 @@
   </si>
   <si>
     <t>length</t>
-  </si>
-  <si>
-    <t>sender first_name</t>
-  </si>
-  <si>
-    <t>sender last name</t>
   </si>
   <si>
     <t>recipient first_name</t>
@@ -202,8 +177,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,12 +222,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF212529"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -281,7 +250,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -306,9 +275,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -625,33 +591,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EE8AA69-184F-4EDD-986D-80D10476D1BA}">
-  <dimension ref="A1:AF20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AA6" sqref="AA6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="34.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" customWidth="1"/>
-    <col min="5" max="12" width="15.6640625" customWidth="1"/>
-    <col min="13" max="13" width="15.6640625" style="10" customWidth="1"/>
-    <col min="14" max="16" width="15.6640625" customWidth="1"/>
-    <col min="17" max="17" width="20.109375" style="10" customWidth="1"/>
-    <col min="18" max="19" width="15.6640625" customWidth="1"/>
-    <col min="20" max="20" width="20.88671875" customWidth="1"/>
-    <col min="21" max="28" width="15.6640625" customWidth="1"/>
-    <col min="29" max="29" width="25.88671875" customWidth="1"/>
-    <col min="30" max="30" width="21" style="10" customWidth="1"/>
-    <col min="31" max="31" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" style="10" customWidth="1"/>
+    <col min="14" max="15" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="20.85546875" customWidth="1"/>
+    <col min="17" max="24" width="15.7109375" customWidth="1"/>
+    <col min="25" max="25" width="25.85546875" customWidth="1"/>
+    <col min="26" max="26" width="21" style="10" customWidth="1"/>
+    <col min="27" max="27" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -668,7 +632,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
@@ -677,13 +641,13 @@
         <v>5</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>7</v>
@@ -692,69 +656,57 @@
         <v>8</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="X1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="B2" t="s">
         <v>18</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
       </c>
       <c r="C2">
         <v>29873928</v>
@@ -775,132 +727,120 @@
         <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="P2">
+        <v>28937</v>
+      </c>
+      <c r="Q2">
+        <v>87272</v>
+      </c>
+      <c r="R2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="S2" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="T2" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="R2" t="s">
-        <v>25</v>
-      </c>
-      <c r="T2">
-        <v>28937</v>
-      </c>
       <c r="U2">
-        <v>87272</v>
-      </c>
-      <c r="V2" t="s">
-        <v>26</v>
-      </c>
-      <c r="W2" t="s">
+        <v>98273982783</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>5</v>
+      </c>
+      <c r="Y2" t="s">
         <v>27</v>
       </c>
-      <c r="X2" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y2">
-        <v>98273982783</v>
-      </c>
-      <c r="AA2">
-        <v>1</v>
-      </c>
-      <c r="AB2">
-        <v>5</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AD2" s="10">
+      <c r="Z2" s="10">
         <v>233847</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>123</v>
       </c>
       <c r="F3" s="1"/>
       <c r="L3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="AA3">
+      <c r="W3">
         <v>2</v>
       </c>
-      <c r="AB3">
+      <c r="X3">
         <v>1</v>
       </c>
-      <c r="AC3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AD3" s="10">
+      <c r="Y3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z3" s="10">
         <v>233848</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>123</v>
       </c>
       <c r="F4" s="1"/>
       <c r="L4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="AA4">
+      <c r="W4">
         <v>1</v>
       </c>
-      <c r="AB4">
+      <c r="X4">
         <v>2</v>
       </c>
-      <c r="AC4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD4" s="10">
+      <c r="Y4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z4" s="10">
         <v>233884</v>
       </c>
-      <c r="AE4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AA4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>123</v>
       </c>
       <c r="F5" s="1"/>
       <c r="L5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="AA5">
+      <c r="W5">
         <v>1</v>
       </c>
-      <c r="AB5">
+      <c r="X5">
         <v>1</v>
       </c>
-      <c r="AC5" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD5" s="10">
+      <c r="Y5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z5" s="10">
         <v>398744</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D6">
         <v>124</v>
@@ -918,221 +858,196 @@
         <v>23</v>
       </c>
       <c r="I6" t="s">
-        <v>53</v>
-      </c>
-      <c r="K6" t="s">
-        <v>36</v>
+        <v>45</v>
+      </c>
+      <c r="J6" t="s">
+        <v>32</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6" s="10">
-        <v>2938998</v>
+        <v>33</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="N6" t="s">
-        <v>38</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q6" s="10" t="s">
-        <v>55</v>
+        <v>34</v>
+      </c>
+      <c r="P6">
+        <v>2323</v>
+      </c>
+      <c r="Q6">
+        <v>23243</v>
       </c>
       <c r="R6" t="s">
-        <v>40</v>
-      </c>
-      <c r="T6">
-        <v>2323</v>
+        <v>35</v>
+      </c>
+      <c r="S6" t="s">
+        <v>23</v>
+      </c>
+      <c r="T6" t="s">
+        <v>24</v>
       </c>
       <c r="U6">
-        <v>23243</v>
-      </c>
-      <c r="V6" t="s">
+        <v>82973987</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>2</v>
+      </c>
+      <c r="Y6" t="s">
         <v>41</v>
       </c>
-      <c r="W6" t="s">
-        <v>27</v>
-      </c>
-      <c r="X6" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y6">
-        <v>82973987</v>
-      </c>
-      <c r="AA6">
-        <v>1</v>
-      </c>
-      <c r="AB6">
-        <v>2</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD6" s="10">
+      <c r="Z6" s="10">
         <v>983434</v>
       </c>
-      <c r="AF6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AB6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="L7" s="2"/>
-      <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="L8" s="2"/>
-      <c r="P8" s="2"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="L9" s="2"/>
-      <c r="P9" s="2"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="L10" s="2"/>
-      <c r="P10" s="2"/>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="L11" s="2"/>
-      <c r="P11" s="2"/>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="L12" s="2"/>
-      <c r="P12" s="2"/>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="L13" s="2"/>
-      <c r="P13" s="2"/>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="L14" s="2"/>
-      <c r="P14" s="2"/>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="L15" s="2"/>
-      <c r="P15" s="2"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="L16" s="2"/>
-      <c r="P16" s="2"/>
-    </row>
-    <row r="17" spans="12:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L17" s="2"/>
-      <c r="P17" s="2"/>
-    </row>
-    <row r="18" spans="12:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L18" s="2"/>
-      <c r="P18" s="2"/>
-    </row>
-    <row r="19" spans="12:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L19" s="2"/>
-      <c r="P19" s="2"/>
-    </row>
-    <row r="20" spans="12:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L20" s="2"/>
-      <c r="P20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE2:AF4" xr:uid="{5EA4B698-AE3D-433F-8CDD-F6223315DA05}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2:AB4">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{94C1A35A-BA51-4B20-A483-4390B8EE37CA}"/>
-    <hyperlink ref="P2" r:id="rId2" xr:uid="{2624B40A-BD9F-4C8E-9E98-9D8E2F333CFA}"/>
-    <hyperlink ref="L6" r:id="rId3" xr:uid="{BA23395B-4CA3-4709-9BE2-0437065D5169}"/>
-    <hyperlink ref="P6" r:id="rId4" xr:uid="{BF50404B-E00C-488C-BAE6-C42EFF0CBD20}"/>
+    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="L6" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CD93335-3AF0-44B7-948E-2C501CF121F2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="e">
         <f>Sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>Sheet1!B1</f>
         <v>carrier</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>Sheet1!B2</f>
         <v>fedex</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>Sheet1!B3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>Sheet1!B4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>Sheet1!B5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>Sheet1!B6</f>
         <v>kjsadb</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="e">
         <f>Sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="e">
         <f>Sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="e">
         <f>Sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="e">
         <f>Sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="e">
         <f>Sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="e">
         <f>Sheet1!#REF!</f>
         <v>#REF!</v>

</xml_diff>

<commit_message>
Product and Order Inventory Test
</commit_message>
<xml_diff>
--- a/public/uploads/order-import.xlsx
+++ b/public/uploads/order-import.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\hd-v2\public\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hd-v2\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FFDB28-D4E7-4780-B65D-AD33828A0CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>merchant</t>
   </si>
@@ -93,9 +104,6 @@
     <t>some address</t>
   </si>
   <si>
-    <t>sjnd</t>
-  </si>
-  <si>
     <t>SP</t>
   </si>
   <si>
@@ -108,21 +116,9 @@
     <t>NCM</t>
   </si>
   <si>
-    <t>soccer ball</t>
-  </si>
-  <si>
     <t>product quantity</t>
   </si>
   <si>
-    <t>kjasbd</t>
-  </si>
-  <si>
-    <t>kjsadb</t>
-  </si>
-  <si>
-    <t>kalsdn</t>
-  </si>
-  <si>
     <t>kjasbdjb</t>
   </si>
   <si>
@@ -132,9 +128,6 @@
     <t>sakjdsd</t>
   </si>
   <si>
-    <t>asdfjsan</t>
-  </si>
-  <si>
     <t>length</t>
   </si>
   <si>
@@ -153,9 +146,6 @@
     <t>battery</t>
   </si>
   <si>
-    <t>shoes</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -172,12 +162,45 @@
   </si>
   <si>
     <t>Freight To Custom</t>
+  </si>
+  <si>
+    <t>SKU</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>usps</t>
+  </si>
+  <si>
+    <t>Racing Car</t>
+  </si>
+  <si>
+    <t>A5 Cell</t>
+  </si>
+  <si>
+    <t>Charger</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Santos</t>
+  </si>
+  <si>
+    <t>SKU0024</t>
+  </si>
+  <si>
+    <t>SKU0023</t>
+  </si>
+  <si>
+    <t>SKU0022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -250,7 +273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -270,7 +293,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -591,31 +613,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AD19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD6" sqref="AD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="12" width="15.7109375" customWidth="1"/>
-    <col min="13" max="13" width="20.140625" style="10" customWidth="1"/>
-    <col min="14" max="15" width="15.7109375" customWidth="1"/>
-    <col min="16" max="16" width="20.85546875" customWidth="1"/>
-    <col min="17" max="24" width="15.7109375" customWidth="1"/>
-    <col min="25" max="25" width="25.85546875" customWidth="1"/>
-    <col min="26" max="26" width="21" style="10" customWidth="1"/>
-    <col min="27" max="27" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="34.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="12" width="15.6640625" customWidth="1"/>
+    <col min="13" max="13" width="20.109375" style="9" customWidth="1"/>
+    <col min="14" max="15" width="15.6640625" customWidth="1"/>
+    <col min="16" max="16" width="20.88671875" customWidth="1"/>
+    <col min="17" max="24" width="15.6640625" customWidth="1"/>
+    <col min="25" max="25" width="25.88671875" customWidth="1"/>
+    <col min="26" max="26" width="21" style="9" customWidth="1"/>
+    <col min="27" max="27" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -632,7 +654,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
@@ -641,18 +663,18 @@
         <v>5</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>8</v>
       </c>
       <c r="N1" s="3" t="s">
@@ -680,28 +702,34 @@
         <v>16</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="Y1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="9" t="s">
-        <v>26</v>
-      </c>
       <c r="AA1" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="AB1" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
@@ -712,12 +740,12 @@
         <v>29873928</v>
       </c>
       <c r="D2">
-        <v>123</v>
+        <v>2455</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2">
         <v>12</v>
       </c>
       <c r="G2">
@@ -727,7 +755,7 @@
         <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J2" t="s">
         <v>19</v>
@@ -735,8 +763,8 @@
       <c r="L2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="10" t="s">
-        <v>46</v>
+      <c r="M2" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="N2" t="s">
         <v>21</v>
@@ -748,217 +776,222 @@
         <v>87272</v>
       </c>
       <c r="R2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S2" t="s">
         <v>22</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>23</v>
-      </c>
-      <c r="T2" t="s">
-        <v>24</v>
       </c>
       <c r="U2">
         <v>98273982783</v>
       </c>
       <c r="W2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="X2">
         <v>5</v>
       </c>
       <c r="Y2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z2" s="10">
+        <v>45</v>
+      </c>
+      <c r="Z2" s="9">
         <v>233847</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD2">
+        <v>30203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D3">
-        <v>123</v>
+        <v>2455</v>
       </c>
       <c r="F3" s="1"/>
       <c r="L3" s="2"/>
       <c r="W3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="X3">
         <v>1</v>
       </c>
       <c r="Y3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z3" s="10">
+        <v>46</v>
+      </c>
+      <c r="Z3" s="9">
         <v>233848</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD3">
+        <v>30202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D4">
-        <v>123</v>
+        <v>2455</v>
       </c>
       <c r="F4" s="1"/>
       <c r="L4" s="2"/>
       <c r="W4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="X4">
         <v>2</v>
       </c>
       <c r="Y4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z4" s="9">
+        <v>233884</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD4">
+        <v>30201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5">
+        <v>30065626894</v>
+      </c>
+      <c r="D5">
+        <v>2456</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>23</v>
+      </c>
+      <c r="H5">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="Z4" s="10">
-        <v>233884</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="D5">
-        <v>123</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="L5" s="2"/>
+      <c r="N5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5">
+        <v>2323</v>
+      </c>
+      <c r="Q5">
+        <v>23243</v>
+      </c>
+      <c r="R5" t="s">
+        <v>48</v>
+      </c>
+      <c r="S5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U5">
+        <v>82973987</v>
+      </c>
       <c r="W5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="X5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y5" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z5" s="10">
-        <v>398744</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6">
-        <v>124</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="8">
-        <v>2</v>
-      </c>
-      <c r="G6">
-        <v>23</v>
-      </c>
-      <c r="H6">
-        <v>23</v>
-      </c>
-      <c r="I6" t="s">
         <v>45</v>
       </c>
-      <c r="J6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="N6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P6">
-        <v>2323</v>
-      </c>
-      <c r="Q6">
-        <v>23243</v>
-      </c>
-      <c r="R6" t="s">
-        <v>35</v>
-      </c>
-      <c r="S6" t="s">
-        <v>23</v>
-      </c>
-      <c r="T6" t="s">
-        <v>24</v>
-      </c>
-      <c r="U6">
-        <v>82973987</v>
-      </c>
-      <c r="W6">
-        <v>1</v>
-      </c>
-      <c r="X6">
-        <v>2</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z6" s="10">
+      <c r="Z5" s="9">
         <v>983434</v>
       </c>
-      <c r="AB6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="AB5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD5">
+        <v>30203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L19" s="2"/>
-    </row>
-    <row r="20" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2:AB4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2:AB4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-    <hyperlink ref="L6" r:id="rId2"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="L5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -966,88 +999,88 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="e">
         <f>Sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>Sheet1!B1</f>
         <v>carrier</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>Sheet1!B2</f>
         <v>fedex</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>Sheet1!B3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>Sheet1!B4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="e">
+        <f>Sheet1!#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
         <f>Sheet1!B5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="str">
-        <f>Sheet1!B6</f>
-        <v>kjsadb</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>usps</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="e">
         <f>Sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="e">
         <f>Sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="e">
         <f>Sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="e">
         <f>Sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="e">
         <f>Sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="e">
         <f>Sheet1!#REF!</f>
         <v>#REF!</v>

</xml_diff>

<commit_message>
Order Import Sample File Update
</commit_message>
<xml_diff>
--- a/public/uploads/order-import.xlsx
+++ b/public/uploads/order-import.xlsx
@@ -1,24 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\hd-v2\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D3A8CB-EF1E-48D9-83F0-275A4F501436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -183,7 +195,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -601,31 +613,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="12" width="15.7109375" customWidth="1"/>
-    <col min="13" max="13" width="20.140625" style="10" customWidth="1"/>
-    <col min="14" max="15" width="15.7109375" customWidth="1"/>
-    <col min="16" max="16" width="20.85546875" customWidth="1"/>
-    <col min="17" max="24" width="15.7109375" customWidth="1"/>
-    <col min="25" max="25" width="25.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="34.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="12" width="15.6640625" customWidth="1"/>
+    <col min="13" max="13" width="20.109375" style="10" customWidth="1"/>
+    <col min="14" max="15" width="15.6640625" customWidth="1"/>
+    <col min="16" max="16" width="20.88671875" customWidth="1"/>
+    <col min="17" max="24" width="15.6640625" customWidth="1"/>
+    <col min="25" max="25" width="25.88671875" customWidth="1"/>
     <col min="26" max="26" width="21" style="10" customWidth="1"/>
-    <col min="27" max="27" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -705,10 +717,10 @@
         <v>25</v>
       </c>
       <c r="AA1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB1" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="AC1" s="12" t="s">
         <v>47</v>
@@ -717,7 +729,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
@@ -788,7 +800,7 @@
         <v>233847</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D3">
         <v>123</v>
       </c>
@@ -807,7 +819,7 @@
         <v>233848</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D4">
         <v>123</v>
       </c>
@@ -829,7 +841,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="D5">
         <v>123</v>
       </c>
@@ -848,7 +860,7 @@
         <v>398744</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>28</v>
       </c>
@@ -922,59 +934,59 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2:AB4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2:AB4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-    <hyperlink ref="L6" r:id="rId2"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="L6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -982,88 +994,88 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="e">
         <f>Sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>Sheet1!B1</f>
         <v>carrier</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>Sheet1!B2</f>
         <v>fedex</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>Sheet1!B3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>Sheet1!B4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>Sheet1!B5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>Sheet1!B6</f>
         <v>kjsadb</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="e">
         <f>Sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="e">
         <f>Sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="e">
         <f>Sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="e">
         <f>Sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="e">
         <f>Sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="e">
         <f>Sheet1!#REF!</f>
         <v>#REF!</v>

</xml_diff>